<commit_message>
Add of SVG draw
</commit_message>
<xml_diff>
--- a/cablage.xlsx
+++ b/cablage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\OneDrive\Bureau\cablage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\OneDrive\Documents\projets\cable_maker_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF360A13-A406-4222-8C67-8A84E18C8D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B5EBB2-5388-46F3-BF14-1F5021F01C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cables" sheetId="3" r:id="rId1"/>
@@ -670,7 +670,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,7 +800,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +858,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1090,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1146,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CF81E09-7BBF-4E8D-96D2-E8E7143C86EF}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>